<commit_message>
model of System generated
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Documents\CPCON\GALERIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Documents\CPCON\GALERIA\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3461B9E3-7C49-4C67-87CA-B01A7D15373F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC727BC-7805-4C1B-9869-DAF3C64AB65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F51D8257-F097-4215-AEC6-98FA6048748B}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F51D8257-F097-4215-AEC6-98FA6048748B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Estabelecimento</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Valor de Custo Unitario</t>
+  </si>
+  <si>
+    <t>CONTA ORIGEM</t>
+  </si>
+  <si>
+    <t>DESC CONTA ORIGEM</t>
+  </si>
+  <si>
+    <t>AQUISITION ORIGEM</t>
+  </si>
+  <si>
+    <t>INFO</t>
   </si>
 </sst>
 </file>
@@ -163,16 +175,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42843F48-4077-42E1-A5B5-609320B8C7FA}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="O1" sqref="O1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,9 +520,11 @@
     <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,8 +567,17 @@
       <c r="N1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -586,8 +610,17 @@
       <c r="N2" s="3">
         <v>0</v>
       </c>
+      <c r="O2" s="1">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>41255</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>